<commit_message>
Jul active DPs upload
</commit_message>
<xml_diff>
--- a/H2coco/PO.xlsx
+++ b/H2coco/PO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Github/XeroAPI/dashboardWebsite/backend/uploads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Github/XeroAPI/H2coco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C904138-1B22-7B4A-9A4F-B24F8CF0FCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7777F978-A125-7345-B8A7-FFE011312CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" xr2:uid="{4B9AE9D0-272D-6147-B144-109295B6F9E3}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:J997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,251 +503,251 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3991</v>
+        <v>4107</v>
       </c>
       <c r="B4" s="3">
-        <v>45784</v>
+        <v>45813</v>
       </c>
       <c r="C4" s="2">
-        <v>0.61570000000000003</v>
+        <v>0.64966999999999997</v>
       </c>
       <c r="D4" s="6">
-        <v>7603.2</v>
+        <v>7054.9</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4058</v>
+        <v>4112</v>
       </c>
       <c r="B5" s="3">
-        <v>45799</v>
+        <v>45813</v>
       </c>
       <c r="C5" s="2">
-        <v>0.64217000000000002</v>
+        <v>0.64966999999999997</v>
       </c>
       <c r="D5" s="6">
-        <v>4276.74</v>
+        <v>7350</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>4059</v>
+        <v>4062</v>
       </c>
       <c r="B6" s="3">
-        <v>45799</v>
+        <v>45813</v>
       </c>
       <c r="C6" s="2">
-        <v>0.64217000000000002</v>
+        <v>0.65178000000000003</v>
       </c>
       <c r="D6" s="6">
-        <v>4616.49</v>
+        <v>3801.6</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4072</v>
+        <v>4140</v>
       </c>
       <c r="B7" s="3">
-        <v>45799</v>
+        <v>45819</v>
       </c>
       <c r="C7" s="2">
-        <v>0.64217000000000002</v>
+        <v>0.65086999999999995</v>
       </c>
       <c r="D7" s="6">
-        <v>4143.4799999999996</v>
+        <v>7916.25</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>4087</v>
+        <v>4144</v>
       </c>
       <c r="B8" s="3">
-        <v>45799</v>
+        <v>45819</v>
       </c>
       <c r="C8" s="2">
-        <v>0.64217000000000002</v>
+        <v>0.65086999999999995</v>
       </c>
       <c r="D8" s="6">
-        <v>4616.49</v>
+        <v>7350</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>4047</v>
+        <v>4090</v>
       </c>
       <c r="B9" s="3">
-        <v>45799</v>
+        <v>45828</v>
       </c>
       <c r="C9" s="2">
-        <v>0.64764999999999995</v>
+        <v>0.64754999999999996</v>
       </c>
       <c r="D9" s="6">
-        <v>7603.2</v>
+        <v>8316</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>4048</v>
+        <v>4122</v>
       </c>
       <c r="B10" s="3">
-        <v>45799</v>
+        <v>45828</v>
       </c>
       <c r="C10" s="2">
-        <v>0.64265000000000005</v>
+        <v>0.64720999999999995</v>
       </c>
       <c r="D10" s="6">
-        <v>3801.6</v>
+        <v>3979.95</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>4050</v>
+        <v>4153</v>
       </c>
       <c r="B11" s="3">
-        <v>45799</v>
+        <v>45828</v>
       </c>
       <c r="C11" s="2">
-        <v>0.64764999999999995</v>
+        <v>0.64720999999999995</v>
       </c>
       <c r="D11" s="6">
-        <v>7603.2</v>
+        <v>3979.95</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>4033</v>
+        <v>4166</v>
       </c>
       <c r="B12" s="3">
-        <v>45806</v>
+        <v>45828</v>
       </c>
       <c r="C12" s="2">
-        <v>0.64151000000000002</v>
+        <v>0.64754999999999996</v>
       </c>
       <c r="D12" s="6">
-        <v>5400</v>
+        <v>3967.5</v>
       </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>4057</v>
+        <v>4168</v>
       </c>
       <c r="B13" s="3">
-        <v>45806</v>
+        <v>45828</v>
       </c>
       <c r="C13" s="2">
-        <v>0.64151000000000002</v>
+        <v>0.64754999999999996</v>
       </c>
       <c r="D13" s="6">
-        <v>4101.45</v>
+        <v>3967.5</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>4107</v>
+        <v>4195</v>
       </c>
       <c r="B14" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C14" s="2">
-        <v>0.64966999999999997</v>
+        <v>0.64754999999999996</v>
       </c>
       <c r="D14" s="6">
-        <v>7054.9</v>
+        <v>4428</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>4109</v>
+        <v>4199</v>
       </c>
       <c r="B15" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C15" s="2">
-        <v>0.64966999999999997</v>
+        <v>0.64754999999999996</v>
       </c>
       <c r="D15" s="6">
-        <v>7127.9</v>
+        <v>4066.2</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>4112</v>
+        <v>4124</v>
       </c>
       <c r="B16" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C16" s="2">
-        <v>0.64966999999999997</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D16" s="6">
-        <v>7350</v>
+        <v>3801.6</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>4103</v>
+        <v>4125</v>
       </c>
       <c r="B17" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C17" s="2">
-        <v>0.61592999999999998</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D17" s="6">
-        <v>2254.5</v>
+        <v>3801.6</v>
       </c>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>4138</v>
+        <v>4126</v>
       </c>
       <c r="B18" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C18" s="2">
-        <v>0.61592999999999998</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D18" s="6">
-        <v>3801.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>4139</v>
+        <v>4156</v>
       </c>
       <c r="B19" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C19" s="2">
-        <v>0.61592999999999998</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D19" s="6">
-        <v>4455</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>4062</v>
+        <v>4157</v>
       </c>
       <c r="B20" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C20" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D20" s="6">
         <v>3801.6</v>
@@ -755,13 +755,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>4063</v>
+        <v>4159</v>
       </c>
       <c r="B21" s="3">
-        <v>45813</v>
+        <v>45828</v>
       </c>
       <c r="C21" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.64898999999999996</v>
       </c>
       <c r="D21" s="6">
         <v>3801.6</v>
@@ -769,573 +769,573 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>4064</v>
+        <v>4170</v>
       </c>
       <c r="B22" s="3">
-        <v>45813</v>
+        <v>45834</v>
       </c>
       <c r="C22" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.61589000000000005</v>
       </c>
       <c r="D22" s="6">
-        <v>3801.6</v>
+        <v>7127.9</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>4074</v>
+        <v>4197</v>
       </c>
       <c r="B23" s="3">
-        <v>45813</v>
+        <v>45834</v>
       </c>
       <c r="C23" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.61589000000000005</v>
       </c>
       <c r="D23" s="6">
-        <v>3801.6</v>
+        <v>7916.25</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>4075</v>
+        <v>4198</v>
       </c>
       <c r="B24" s="3">
-        <v>45813</v>
+        <v>45834</v>
       </c>
       <c r="C24" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.61589000000000005</v>
       </c>
       <c r="D24" s="6">
-        <v>3801.6</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>4076</v>
+        <v>4200</v>
       </c>
       <c r="B25" s="3">
-        <v>45813</v>
+        <v>45834</v>
       </c>
       <c r="C25" s="2">
-        <v>0.65178000000000003</v>
+        <v>0.61589000000000005</v>
       </c>
       <c r="D25" s="6">
-        <v>3801.6</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>4140</v>
+        <v>4221</v>
       </c>
       <c r="B26" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C26" s="2">
-        <v>0.65086999999999995</v>
+        <v>0.61580000000000001</v>
       </c>
       <c r="D26" s="6">
-        <v>7916.25</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>4142</v>
+        <v>4118</v>
       </c>
       <c r="B27" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C27" s="2">
-        <v>0.65086999999999995</v>
+        <v>0.65142</v>
       </c>
       <c r="D27" s="6">
-        <v>7350</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>4144</v>
+        <v>4119</v>
       </c>
       <c r="B28" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C28" s="2">
-        <v>0.65086999999999995</v>
+        <v>0.65142</v>
       </c>
       <c r="D28" s="6">
-        <v>7350</v>
+        <v>4201.2</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>4146</v>
+        <v>4120</v>
       </c>
       <c r="B29" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C29" s="2">
-        <v>0.65086999999999995</v>
+        <v>0.65142</v>
       </c>
       <c r="D29" s="6">
-        <v>7350</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>4070</v>
+        <v>4121</v>
       </c>
       <c r="B30" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C30" s="2">
-        <v>0.65042</v>
+        <v>0.65142</v>
       </c>
       <c r="D30" s="6">
-        <v>4252.5</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>4071</v>
+        <v>4148</v>
       </c>
       <c r="B31" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C31" s="2">
-        <v>0.65042</v>
+        <v>0.65142</v>
       </c>
       <c r="D31" s="6">
-        <v>3888.15</v>
+        <v>4241.7</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>4115</v>
+        <v>4150</v>
       </c>
       <c r="B32" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C32" s="2">
-        <v>0.65042</v>
+        <v>0.65142</v>
       </c>
       <c r="D32" s="6">
-        <v>4158</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>4116</v>
+        <v>4151</v>
       </c>
       <c r="B33" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C33" s="2">
-        <v>0.65042</v>
+        <v>0.65142</v>
       </c>
       <c r="D33" s="6">
-        <v>4293</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>4117</v>
+        <v>4152</v>
       </c>
       <c r="B34" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C34" s="2">
-        <v>0.65042</v>
-      </c>
-      <c r="D34" s="5">
-        <v>4066.2</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D34" s="6">
+        <v>3801.9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>4137</v>
+        <v>4167</v>
       </c>
       <c r="B35" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C35" s="2">
-        <v>0.65042</v>
-      </c>
-      <c r="D35" s="5">
-        <v>4293</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D35" s="6">
+        <v>15870</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>4141</v>
+        <v>4169</v>
       </c>
       <c r="B36" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C36" s="2">
-        <v>0.65042</v>
-      </c>
-      <c r="D36" s="5">
-        <v>4114.95</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D36" s="6">
+        <v>7935</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>4095</v>
+        <v>4173</v>
       </c>
       <c r="B37" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C37" s="2">
-        <v>0.65083999999999997</v>
-      </c>
-      <c r="D37" s="5">
-        <v>3801.6</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D37" s="6">
+        <v>7935</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>4096</v>
+        <v>4174</v>
       </c>
       <c r="B38" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C38" s="2">
-        <v>0.65083999999999997</v>
-      </c>
-      <c r="D38" s="5">
-        <v>3801.6</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D38" s="6">
+        <v>3884.7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>4097</v>
+        <v>4196</v>
       </c>
       <c r="B39" s="3">
-        <v>45819</v>
+        <v>45834</v>
       </c>
       <c r="C39" s="2">
-        <v>0.65083999999999997</v>
-      </c>
-      <c r="D39" s="5">
-        <v>3801.6</v>
+        <v>0.65142</v>
+      </c>
+      <c r="D39" s="6">
+        <v>4197.75</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>4098</v>
+        <v>4216</v>
       </c>
       <c r="B40" s="3">
-        <v>45819</v>
+        <v>45841</v>
       </c>
       <c r="C40" s="2">
-        <v>0.65083999999999997</v>
-      </c>
-      <c r="D40" s="5">
-        <v>3801.6</v>
+        <v>0.65475000000000005</v>
+      </c>
+      <c r="D40" s="6">
+        <v>7113</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>4068</v>
+        <v>4219</v>
       </c>
       <c r="B41" s="3">
-        <v>45828</v>
+        <v>45841</v>
       </c>
       <c r="C41" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D41" s="5">
-        <v>3979.95</v>
+        <v>0.65475000000000005</v>
+      </c>
+      <c r="D41" s="6">
+        <v>7155.6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>4083</v>
+        <v>4225</v>
       </c>
       <c r="B42" s="3">
-        <v>45828</v>
+        <v>45841</v>
       </c>
       <c r="C42" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D42" s="5">
-        <v>3801.9</v>
+        <v>0.65475000000000005</v>
+      </c>
+      <c r="D42" s="6">
+        <v>7350</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>4084</v>
+        <v>4086</v>
       </c>
       <c r="B43" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C43" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D43" s="5">
-        <v>4455</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D43" s="6">
+        <v>4279.5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>4085</v>
+        <v>4154</v>
       </c>
       <c r="B44" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C44" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D44" s="5">
-        <v>3979.95</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D44" s="6">
+        <v>4293</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>4090</v>
+        <v>4175</v>
       </c>
       <c r="B45" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C45" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D45" s="5">
-        <v>8316</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3967.5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>4122</v>
+        <v>4203</v>
       </c>
       <c r="B46" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C46" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D46" s="5">
-        <v>3979.95</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D46" s="6">
+        <v>4428</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>4143</v>
+        <v>4205</v>
       </c>
       <c r="B47" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C47" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D47" s="5">
-        <v>4158</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D47" s="6">
+        <v>3979.95</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>4147</v>
+        <v>4206</v>
       </c>
       <c r="B48" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C48" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D48" s="5">
-        <v>3979.95</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D48" s="6">
+        <v>4062.75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>4149</v>
+        <v>4222</v>
       </c>
       <c r="B49" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C49" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D49" s="5">
-        <v>3979.95</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D49" s="6">
+        <v>4158</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>4153</v>
+        <v>4223</v>
       </c>
       <c r="B50" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C50" s="2">
-        <v>0.64720999999999995</v>
-      </c>
-      <c r="D50" s="5">
-        <v>3979.95</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D50" s="6">
+        <v>4158</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>4155</v>
+        <v>4224</v>
       </c>
       <c r="B51" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C51" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D51" s="5">
-        <v>4293</v>
+        <v>0.65356000000000003</v>
+      </c>
+      <c r="D51" s="6">
+        <v>3888.15</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>4165</v>
+        <v>4184</v>
       </c>
       <c r="B52" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C52" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D52" s="5">
-        <v>15870</v>
+        <v>0.65310000000000001</v>
+      </c>
+      <c r="D52" s="6">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>4166</v>
+        <v>4185</v>
       </c>
       <c r="B53" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C53" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D53" s="5">
-        <v>3967.5</v>
+        <v>0.65310000000000001</v>
+      </c>
+      <c r="D53" s="6">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>4168</v>
+        <v>4187</v>
       </c>
       <c r="B54" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C54" s="2">
-        <v>0.64754999999999996</v>
-      </c>
-      <c r="D54" s="5">
-        <v>3967.5</v>
+        <v>0.65310000000000001</v>
+      </c>
+      <c r="D54" s="6">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>4171</v>
+        <v>4188</v>
       </c>
       <c r="B55" s="3">
-        <v>45828</v>
+        <v>45845</v>
       </c>
       <c r="C55" s="2">
-        <v>0.64754999999999996</v>
+        <v>0.65310000000000001</v>
       </c>
       <c r="D55" s="5">
-        <v>3801.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>4195</v>
+        <v>4218</v>
       </c>
       <c r="B56" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C56" s="2">
-        <v>0.64754999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D56" s="5">
-        <v>4428</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>4199</v>
+        <v>4246</v>
       </c>
       <c r="B57" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C57" s="2">
-        <v>0.64754999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D57" s="5">
-        <v>4066.2</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>4124</v>
+        <v>4265</v>
       </c>
       <c r="B58" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C58" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D58" s="5">
-        <v>3801.6</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>4125</v>
+        <v>4266</v>
       </c>
       <c r="B59" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C59" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D59" s="5">
-        <v>3801.6</v>
+        <v>7127.9</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>4126</v>
+        <v>4286</v>
       </c>
       <c r="B60" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C60" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D60" s="5">
-        <v>3801.6</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>4156</v>
+        <v>4287</v>
       </c>
       <c r="B61" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C61" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65354000000000001</v>
       </c>
       <c r="D61" s="5">
-        <v>3801.6</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>4157</v>
+        <v>4235</v>
       </c>
       <c r="B62" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C62" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65380000000000005</v>
       </c>
       <c r="D62" s="5">
         <v>3801.6</v>
@@ -1343,13 +1343,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>4158</v>
+        <v>4236</v>
       </c>
       <c r="B63" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C63" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65380000000000005</v>
       </c>
       <c r="D63" s="5">
         <v>3801.6</v>
@@ -1357,13 +1357,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>4159</v>
+        <v>4237</v>
       </c>
       <c r="B64" s="3">
-        <v>45828</v>
+        <v>45848</v>
       </c>
       <c r="C64" s="2">
-        <v>0.64898999999999996</v>
+        <v>0.65380000000000005</v>
       </c>
       <c r="D64" s="5">
         <v>3801.6</v>
@@ -1371,125 +1371,125 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>4170</v>
+        <v>4238</v>
       </c>
       <c r="B65" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C65" s="2">
-        <v>0.61589000000000005</v>
+        <v>0.65380000000000005</v>
       </c>
       <c r="D65" s="5">
-        <v>7127.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>4172</v>
+        <v>4176</v>
       </c>
       <c r="B66" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C66" s="2">
-        <v>0.61589000000000005</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D66" s="5">
-        <v>7054.9</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>4197</v>
+        <v>4177</v>
       </c>
       <c r="B67" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C67" s="2">
-        <v>0.61589000000000005</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D67" s="5">
-        <v>7916.25</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>4198</v>
+        <v>4180</v>
       </c>
       <c r="B68" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C68" s="2">
-        <v>0.61589000000000005</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D68" s="5">
-        <v>7350</v>
+        <v>3970.95</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>4200</v>
+        <v>4201</v>
       </c>
       <c r="B69" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C69" s="2">
-        <v>0.61589000000000005</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D69" s="5">
-        <v>7350</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>4091</v>
+        <v>4207</v>
       </c>
       <c r="B70" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C70" s="2">
-        <v>0.61580000000000001</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D70" s="5">
-        <v>3801.6</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>4092</v>
+        <v>4208</v>
       </c>
       <c r="B71" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C71" s="2">
-        <v>0.61580000000000001</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D71" s="5">
-        <v>3801.6</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>4221</v>
+        <v>4209</v>
       </c>
       <c r="B72" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C72" s="2">
-        <v>0.61580000000000001</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D72" s="5">
-        <v>3801.6</v>
+        <v>4184.25</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>4118</v>
+        <v>4210</v>
       </c>
       <c r="B73" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C73" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D73" s="5">
         <v>4158</v>
@@ -1497,285 +1497,381 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>4119</v>
+        <v>4217</v>
       </c>
       <c r="B74" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C74" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D74" s="5">
-        <v>4201.2</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>4120</v>
+        <v>4227</v>
       </c>
       <c r="B75" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C75" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D75" s="5">
-        <v>4455</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>4121</v>
+        <v>4228</v>
       </c>
       <c r="B76" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C76" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D76" s="5">
-        <v>4293</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>4148</v>
+        <v>4229</v>
       </c>
       <c r="B77" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C77" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D77" s="5">
-        <v>4241.7</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>4150</v>
+        <v>4230</v>
       </c>
       <c r="B78" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C78" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D78" s="5">
-        <v>3979.95</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>4151</v>
+        <v>1</v>
       </c>
       <c r="B79" s="3">
-        <v>45834</v>
+        <v>45854</v>
       </c>
       <c r="C79" s="2">
-        <v>0.65142</v>
+        <v>0.65175000000000005</v>
       </c>
       <c r="D79" s="5">
-        <v>4158</v>
+        <v>11025</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>4152</v>
+        <v>2</v>
       </c>
       <c r="B80" s="3">
-        <v>45834</v>
+        <v>45854</v>
       </c>
       <c r="C80" s="2">
-        <v>0.65142</v>
+        <v>0.65176000000000001</v>
       </c>
       <c r="D80" s="5">
-        <v>3801.9</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>4167</v>
+        <v>4253</v>
       </c>
       <c r="B81" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C81" s="2">
-        <v>0.65142</v>
+        <v>0.629</v>
       </c>
       <c r="D81" s="5">
-        <v>15870</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>4169</v>
+        <v>4255</v>
       </c>
       <c r="B82" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C82" s="2">
-        <v>0.65142</v>
+        <v>0.629</v>
       </c>
       <c r="D82" s="5">
-        <v>7935</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>4173</v>
+        <v>4258</v>
       </c>
       <c r="B83" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C83" s="2">
-        <v>0.65142</v>
+        <v>0.629</v>
       </c>
       <c r="D83" s="5">
-        <v>7935</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4174</v>
+        <v>4259</v>
       </c>
       <c r="B84" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C84" s="2">
-        <v>0.65142</v>
+        <v>0.629</v>
       </c>
       <c r="D84" s="5">
-        <v>3884.7</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4181</v>
+        <v>4179</v>
       </c>
       <c r="B85" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C85" s="2">
-        <v>0.65142</v>
+        <v>0.65678000000000003</v>
       </c>
       <c r="D85" s="5">
-        <v>4158</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>4196</v>
+        <v>4202</v>
       </c>
       <c r="B86" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C86" s="2">
-        <v>0.65142</v>
+        <v>0.65678000000000003</v>
       </c>
       <c r="D86" s="5">
-        <v>4197.75</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>4226</v>
+        <v>4204</v>
       </c>
       <c r="B87" s="3">
-        <v>45834</v>
+        <v>45855</v>
       </c>
       <c r="C87" s="2">
-        <v>0.65142</v>
+        <v>0.65780000000000005</v>
       </c>
       <c r="D87" s="5">
-        <v>4158</v>
+        <v>4197.75</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
+        <v>4211</v>
+      </c>
+      <c r="B88" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D88" s="5">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>4212</v>
+      </c>
+      <c r="B89" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D89" s="5">
+        <v>4157.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>4214</v>
+      </c>
+      <c r="B90" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D90" s="5">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>4215</v>
+      </c>
+      <c r="B91" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D91" s="5">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>4268</v>
+      </c>
+      <c r="B92" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D92" s="5">
+        <v>3801.9</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>4274</v>
+      </c>
+      <c r="B93" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D93" s="5">
+        <v>4293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>4213</v>
+      </c>
+      <c r="B94" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D94" s="5">
+        <v>3967.5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>4249</v>
+      </c>
+      <c r="B95" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D95" s="5">
+        <v>4455</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>4267</v>
+      </c>
+      <c r="B96" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D96" s="5">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>4269</v>
+      </c>
+      <c r="B97" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D97" s="5">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>4285</v>
+      </c>
+      <c r="B98" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D98" s="5">
+        <v>4455</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>4220</v>
+      </c>
+      <c r="B99" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.66061000000000003</v>
+      </c>
+      <c r="D99" s="5">
+        <v>3801.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
         <v>4182</v>
       </c>
-      <c r="B88" s="3">
+      <c r="B100" s="3">
         <v>45828</v>
       </c>
-      <c r="C88" s="2">
+      <c r="C100" s="2">
         <v>0.64864999999999995</v>
       </c>
-      <c r="D88" s="5">
+      <c r="D100" s="5">
         <v>4667.2700000000004</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="2"/>
-      <c r="B89" s="3"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="5"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="2"/>
-      <c r="B90" s="3"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="5"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
-      <c r="B91" s="3"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="5"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
-      <c r="B92" s="3"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="5"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
-      <c r="B93" s="3"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="5"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
-      <c r="B94" s="3"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="5"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="5"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="2"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="5"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="2"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="5"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="2"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="5"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="2"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="5"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="2"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2"/>

</xml_diff>

<commit_message>
updated PO file for H2 october
</commit_message>
<xml_diff>
--- a/H2coco/PO.xlsx
+++ b/H2coco/PO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Github/XeroAPI/H2coco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E869979-EA46-4E45-BA8E-86136DF301BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A21942A-2333-D54C-8CF0-5EBB68EB9217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" xr2:uid="{4B9AE9D0-272D-6147-B144-109295B6F9E3}"/>
   </bookViews>
@@ -54,9 +54,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -104,16 +101,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB96091-FFF7-FA49-AAE0-56AC976AE7FD}">
   <dimension ref="A1:J996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
-      <selection activeCell="D119" sqref="D2:D119"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="114" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,1874 +468,2184 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2" s="2">
         <v>4169</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="3">
         <v>45834</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="2">
         <v>0.65142</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>7935</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3" s="2">
         <v>4173</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="3">
         <v>45834</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="2">
         <v>0.65142</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>7935</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>4196</v>
-      </c>
-      <c r="B4" s="8">
-        <v>45834</v>
-      </c>
-      <c r="C4" s="7">
-        <v>0.65142</v>
-      </c>
-      <c r="D4" s="6">
-        <v>4197.75</v>
+      <c r="A4" s="2">
+        <v>4227</v>
+      </c>
+      <c r="B4" s="3">
+        <v>45848</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.62860000000000005</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7603.2</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
-        <v>4180</v>
-      </c>
-      <c r="B5" s="8">
+      <c r="A5" s="2">
+        <v>4228</v>
+      </c>
+      <c r="B5" s="3">
         <v>45848</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="2">
         <v>0.62860000000000005</v>
       </c>
-      <c r="D5" s="6">
-        <v>3970.95</v>
+      <c r="D5" s="5">
+        <v>7603.2</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
-        <v>4227</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="2">
+        <v>4229</v>
+      </c>
+      <c r="B6" s="3">
         <v>45848</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="2">
         <v>0.62860000000000005</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>7603.2</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
-        <v>4228</v>
-      </c>
-      <c r="B7" s="8">
+      <c r="A7" s="2">
+        <v>4230</v>
+      </c>
+      <c r="B7" s="3">
         <v>45848</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="2">
         <v>0.62860000000000005</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>7603.2</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
-        <v>4229</v>
-      </c>
-      <c r="B8" s="8">
-        <v>45848</v>
-      </c>
-      <c r="C8" s="7">
-        <v>0.62860000000000005</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="A8" s="2">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45854</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.65175000000000005</v>
+      </c>
+      <c r="D8" s="5">
+        <v>11025</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45854</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.65176000000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1040</v>
+      </c>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4215</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.65678000000000003</v>
+      </c>
+      <c r="D10" s="5">
+        <v>4293</v>
+      </c>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>4213</v>
+      </c>
+      <c r="B11" s="3">
+        <v>45862</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.65963000000000005</v>
+      </c>
+      <c r="D11" s="5">
+        <v>3967.5</v>
+      </c>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>4296</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45869</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.65669999999999995</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3801.6</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>4178</v>
+      </c>
+      <c r="B13" s="3">
+        <v>45869</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3967.5</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>4251</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45869</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4238.25</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>4270</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45869</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="D15" s="5">
+        <v>4293</v>
+      </c>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>4273</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45869</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.62870000000000004</v>
+      </c>
+      <c r="D16" s="5">
+        <v>3967.5</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>4310</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.62877000000000005</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3801.6</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>4312</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.65251000000000003</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3801.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>4313</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.65251000000000003</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3801.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>4290</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.65739999999999998</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2254.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>4291</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.65739999999999998</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>4301</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.65739999999999998</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>4326</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45876</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.65739999999999998</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4157.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>4362</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="D24" s="5">
         <v>7603.2</v>
       </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
-        <v>4230</v>
-      </c>
-      <c r="B9" s="8">
-        <v>45848</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.62860000000000005</v>
-      </c>
-      <c r="D9" s="6">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>4363</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="D25" s="5">
         <v>7603.2</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
-        <v>1</v>
-      </c>
-      <c r="B10" s="8">
-        <v>45854</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.65175000000000005</v>
-      </c>
-      <c r="D10" s="6">
-        <v>11025</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
-        <v>2</v>
-      </c>
-      <c r="B11" s="8">
-        <v>45854</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0.65176000000000001</v>
-      </c>
-      <c r="D11" s="6">
-        <v>1040</v>
-      </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>4211</v>
-      </c>
-      <c r="B12" s="8">
-        <v>45855</v>
-      </c>
-      <c r="C12" s="7">
-        <v>0.65678000000000003</v>
-      </c>
-      <c r="D12" s="6">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>4364</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="D26" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>4365</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="D27" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>4366</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.629</v>
+      </c>
+      <c r="D28" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
+        <v>4306</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.65759000000000001</v>
+      </c>
+      <c r="D29" s="5">
+        <v>3884.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
+        <v>4349</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.65759000000000001</v>
+      </c>
+      <c r="D30" s="5">
+        <v>4062.75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
+        <v>4409</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45883</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.65764999999999996</v>
+      </c>
+      <c r="D31" s="5">
+        <v>7127.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
+        <v>4234</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D32" s="5">
+        <v>3801.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
+        <v>4329</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D33" s="5">
         <v>4293</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
-        <v>4215</v>
-      </c>
-      <c r="B13" s="8">
-        <v>45855</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0.65678000000000003</v>
-      </c>
-      <c r="D13" s="6">
-        <v>4293</v>
-      </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
-        <v>4253</v>
-      </c>
-      <c r="B14" s="8">
-        <v>45855</v>
-      </c>
-      <c r="C14" s="7">
-        <v>0.629</v>
-      </c>
-      <c r="D14" s="6">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>4330</v>
+      </c>
+      <c r="B34" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D34" s="5">
+        <v>3888.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>4331</v>
+      </c>
+      <c r="B35" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D35" s="5">
+        <v>4062.75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
+        <v>4332</v>
+      </c>
+      <c r="B36" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D36" s="5">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
+        <v>4333</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D37" s="5">
         <v>3801.6</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
-        <v>4255</v>
-      </c>
-      <c r="B15" s="8">
-        <v>45855</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0.629</v>
-      </c>
-      <c r="D15" s="6">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
+        <v>4334</v>
+      </c>
+      <c r="B38" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D38" s="5">
+        <v>3801.9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
+        <v>4336</v>
+      </c>
+      <c r="B39" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D39" s="5">
+        <v>3888.15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
+        <v>4345</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D40" s="5">
+        <v>3885.22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
+        <v>4350</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D41" s="5">
+        <v>3888.15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
+        <v>4353</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D42" s="5">
+        <v>3801.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
+        <v>4358</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D43" s="5">
         <v>3801.6</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
-        <v>4259</v>
-      </c>
-      <c r="B16" s="8">
-        <v>45855</v>
-      </c>
-      <c r="C16" s="7">
-        <v>0.629</v>
-      </c>
-      <c r="D16" s="6">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
+        <v>4361</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D44" s="5">
         <v>3801.6</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
-        <v>4213</v>
-      </c>
-      <c r="B17" s="8">
-        <v>45862</v>
-      </c>
-      <c r="C17" s="7">
-        <v>0.65963000000000005</v>
-      </c>
-      <c r="D17" s="6">
-        <v>3967.5</v>
-      </c>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
-        <v>4275</v>
-      </c>
-      <c r="B18" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C18" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D18" s="6">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
+        <v>4388</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D45" s="5">
+        <v>4101.45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
+        <v>4392</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45890</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.6573</v>
+      </c>
+      <c r="D46" s="5">
+        <v>3884.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>4412</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45897</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D47" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="2">
+        <v>4413</v>
+      </c>
+      <c r="B48" s="3">
+        <v>45897</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D48" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="2">
+        <v>4414</v>
+      </c>
+      <c r="B49" s="3">
+        <v>45897</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D49" s="5">
+        <v>7603.2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="2">
+        <v>4415</v>
+      </c>
+      <c r="B50" s="3">
+        <v>45897</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D50" s="5">
         <v>3801.6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="7">
-        <v>4277</v>
-      </c>
-      <c r="B19" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D19" s="6">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="2">
+        <v>4435</v>
+      </c>
+      <c r="B51" s="3">
+        <v>45897</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D51" s="5">
         <v>3801.6</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="7">
-        <v>4278</v>
-      </c>
-      <c r="B20" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D20" s="6">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="2">
+        <v>4231</v>
+      </c>
+      <c r="B52" s="3">
+        <v>45898</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D52" s="5">
         <v>3801.6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="7">
-        <v>4293</v>
-      </c>
-      <c r="B21" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D21" s="6">
-        <v>7603.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="7">
-        <v>4294</v>
-      </c>
-      <c r="B22" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C22" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D22" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="7">
-        <v>4295</v>
-      </c>
-      <c r="B23" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C23" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D23" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="7">
-        <v>4296</v>
-      </c>
-      <c r="B24" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.65669999999999995</v>
-      </c>
-      <c r="D24" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="7">
-        <v>4178</v>
-      </c>
-      <c r="B25" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C25" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D25" s="6">
-        <v>3967.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="7">
-        <v>4251</v>
-      </c>
-      <c r="B26" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C26" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D26" s="6">
-        <v>4238.25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="7">
-        <v>4270</v>
-      </c>
-      <c r="B27" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C27" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D27" s="6">
-        <v>4293</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="7">
-        <v>4271</v>
-      </c>
-      <c r="B28" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C28" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D28" s="6">
-        <v>3888.15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="7">
-        <v>4272</v>
-      </c>
-      <c r="B29" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D29" s="6">
-        <v>4184.25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="7">
-        <v>4273</v>
-      </c>
-      <c r="B30" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C30" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D30" s="6">
-        <v>3967.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="7">
-        <v>4300</v>
-      </c>
-      <c r="B31" s="8">
-        <v>45869</v>
-      </c>
-      <c r="C31" s="7">
-        <v>0.62870000000000004</v>
-      </c>
-      <c r="D31" s="6">
-        <v>3884.7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="7">
-        <v>4321</v>
-      </c>
-      <c r="B32" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C32" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D32" s="6">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="2">
+        <v>4429</v>
+      </c>
+      <c r="B53" s="3">
+        <v>45898</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D53" s="5">
         <v>7350</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
-        <v>4346</v>
-      </c>
-      <c r="B33" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C33" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D33" s="6">
-        <v>7916.25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="7">
-        <v>4347</v>
-      </c>
-      <c r="B34" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C34" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D34" s="6">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="2">
+        <v>4430</v>
+      </c>
+      <c r="B54" s="3">
+        <v>45898</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D54" s="5">
+        <v>7127.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="2">
+        <v>4431</v>
+      </c>
+      <c r="B55" s="3">
+        <v>45898</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D55" s="4">
+        <v>7127.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="2">
+        <v>4448</v>
+      </c>
+      <c r="B56" s="3">
+        <v>45898</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D56" s="4">
         <v>7350</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="7">
-        <v>4310</v>
-      </c>
-      <c r="B35" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C35" s="7">
-        <v>0.62877000000000005</v>
-      </c>
-      <c r="D35" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="7">
-        <v>4397</v>
-      </c>
-      <c r="B36" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C36" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D36" s="6">
-        <v>7095</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="7">
-        <v>4398</v>
-      </c>
-      <c r="B37" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C37" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D37" s="6">
-        <v>7222.5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
-        <v>4311</v>
-      </c>
-      <c r="B38" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C38" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D38" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
-        <v>4312</v>
-      </c>
-      <c r="B39" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C39" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D39" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
-        <v>4313</v>
-      </c>
-      <c r="B40" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C40" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D40" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="7">
-        <v>4338</v>
-      </c>
-      <c r="B41" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C41" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D41" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="7">
-        <v>4339</v>
-      </c>
-      <c r="B42" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C42" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D42" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="7">
-        <v>4340</v>
-      </c>
-      <c r="B43" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C43" s="7">
-        <v>0.65251000000000003</v>
-      </c>
-      <c r="D43" s="6">
-        <v>3801.6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="7">
-        <v>4247</v>
-      </c>
-      <c r="B44" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C44" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D44" s="6">
-        <v>4293</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="7">
-        <v>4248</v>
-      </c>
-      <c r="B45" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C45" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D45" s="6">
-        <v>3979.95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="7">
-        <v>4250</v>
-      </c>
-      <c r="B46" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C46" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D46" s="6">
-        <v>3967.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="7">
-        <v>4288</v>
-      </c>
-      <c r="B47" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C47" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D47" s="6">
-        <v>3967.5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="7">
-        <v>4289</v>
-      </c>
-      <c r="B48" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C48" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D48" s="6">
-        <v>4238.25</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="7">
-        <v>4290</v>
-      </c>
-      <c r="B49" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C49" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D49" s="6">
-        <v>2254.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="7">
-        <v>4291</v>
-      </c>
-      <c r="B50" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C50" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D50" s="6">
-        <v>3979.95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="7">
-        <v>4301</v>
-      </c>
-      <c r="B51" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C51" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D51" s="6">
-        <v>3979.95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="7">
-        <v>4302</v>
-      </c>
-      <c r="B52" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C52" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D52" s="6">
-        <v>4114.95</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="7">
-        <v>4303</v>
-      </c>
-      <c r="B53" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C53" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D53" s="6">
-        <v>3888.15</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="7">
-        <v>4320</v>
-      </c>
-      <c r="B54" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C54" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D54" s="6">
-        <v>3884.7</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="7">
-        <v>4322</v>
-      </c>
-      <c r="B55" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C55" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D55" s="6">
-        <v>4158</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="7">
-        <v>4323</v>
-      </c>
-      <c r="B56" s="8">
-        <v>45876</v>
-      </c>
-      <c r="C56" s="7">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D56" s="6">
-        <v>4114.95</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>4324</v>
+        <v>4449</v>
       </c>
       <c r="B57" s="3">
-        <v>45876</v>
+        <v>45898</v>
       </c>
       <c r="C57" s="2">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D57" s="5">
-        <v>3884.7</v>
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D57" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>4325</v>
+        <v>4450</v>
       </c>
       <c r="B58" s="3">
-        <v>45876</v>
+        <v>45898</v>
       </c>
       <c r="C58" s="2">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D58" s="5">
-        <v>3979.95</v>
+        <v>0.62894000000000005</v>
+      </c>
+      <c r="D58" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>4326</v>
+        <v>4292</v>
       </c>
       <c r="B59" s="3">
-        <v>45876</v>
+        <v>45898</v>
       </c>
       <c r="C59" s="2">
-        <v>0.65739999999999998</v>
-      </c>
-      <c r="D59" s="5">
-        <v>4157.25</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D59" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>4362</v>
+        <v>4352</v>
       </c>
       <c r="B60" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C60" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D60" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D60" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>4363</v>
+        <v>4354</v>
       </c>
       <c r="B61" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C61" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D61" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D61" s="4">
+        <v>4374</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>4364</v>
+        <v>4355</v>
       </c>
       <c r="B62" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C62" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D62" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D62" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>4365</v>
+        <v>4356</v>
       </c>
       <c r="B63" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C63" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D63" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D63" s="4">
+        <v>3979.95</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>4366</v>
+        <v>4389</v>
       </c>
       <c r="B64" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C64" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D64" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D64" s="4">
+        <v>4066.2</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>4367</v>
+        <v>4390</v>
       </c>
       <c r="B65" s="3">
-        <v>45883</v>
+        <v>45898</v>
       </c>
       <c r="C65" s="2">
-        <v>0.629</v>
-      </c>
-      <c r="D65" s="5">
-        <v>7603.2</v>
+        <v>0.65766999999999998</v>
+      </c>
+      <c r="D65" s="4">
+        <v>3801.9</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>4304</v>
+        <v>4351</v>
       </c>
       <c r="B66" s="3">
-        <v>45883</v>
+        <v>45904</v>
       </c>
       <c r="C66" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D66" s="5">
-        <v>3979.95</v>
+        <v>0.65197000000000005</v>
+      </c>
+      <c r="D66" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>4305</v>
+        <v>4393</v>
       </c>
       <c r="B67" s="3">
-        <v>45883</v>
+        <v>45904</v>
       </c>
       <c r="C67" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D67" s="5">
-        <v>4066.2</v>
+        <v>0.65197000000000005</v>
+      </c>
+      <c r="D67" s="4">
+        <v>3888.15</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>4306</v>
+        <v>4394</v>
       </c>
       <c r="B68" s="3">
-        <v>45883</v>
+        <v>45904</v>
       </c>
       <c r="C68" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D68" s="5">
-        <v>3884.7</v>
+        <v>0.65197000000000005</v>
+      </c>
+      <c r="D68" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>4327</v>
+        <v>4395</v>
       </c>
       <c r="B69" s="3">
-        <v>45883</v>
+        <v>45904</v>
       </c>
       <c r="C69" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D69" s="5">
-        <v>4114.95</v>
+        <v>0.65197000000000005</v>
+      </c>
+      <c r="D69" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>4328</v>
+        <v>4479</v>
       </c>
       <c r="B70" s="3">
-        <v>45883</v>
+        <v>45911</v>
       </c>
       <c r="C70" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D70" s="5">
-        <v>3979.95</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D70" s="4">
+        <v>7127.9</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>4349</v>
+        <v>4480</v>
       </c>
       <c r="B71" s="3">
-        <v>45883</v>
+        <v>45911</v>
       </c>
       <c r="C71" s="2">
-        <v>0.65759000000000001</v>
-      </c>
-      <c r="D71" s="5">
-        <v>4062.75</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D71" s="4">
+        <v>7127.9</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>4409</v>
+        <v>4481</v>
       </c>
       <c r="B72" s="3">
-        <v>45883</v>
+        <v>45911</v>
       </c>
       <c r="C72" s="2">
-        <v>0.65764999999999996</v>
-      </c>
-      <c r="D72" s="5">
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D72" s="4">
         <v>7127.9</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>4410</v>
+        <v>4482</v>
       </c>
       <c r="B73" s="3">
-        <v>45883</v>
+        <v>45911</v>
       </c>
       <c r="C73" s="2">
-        <v>0.65764999999999996</v>
-      </c>
-      <c r="D73" s="5">
-        <v>7054.9</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D73" s="4">
+        <v>6832.8</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>4233</v>
+        <v>4526</v>
       </c>
       <c r="B74" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C74" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D74" s="5">
-        <v>3801.6</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D74" s="4">
+        <v>7146.5</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>4234</v>
+        <v>4528</v>
       </c>
       <c r="B75" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C75" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D75" s="5">
-        <v>3801.6</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D75" s="4">
+        <v>7222.5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>4252</v>
+        <v>4529</v>
       </c>
       <c r="B76" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C76" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D76" s="5">
-        <v>4158</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D76" s="4">
+        <v>7098.25</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>4307</v>
+        <v>4533</v>
       </c>
       <c r="B77" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C77" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D77" s="5">
-        <v>3888.15</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D77" s="4">
+        <v>7127.9</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>4308</v>
+        <v>4534</v>
       </c>
       <c r="B78" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C78" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D78" s="5">
-        <v>4027.14</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D78" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>4309</v>
+        <v>4536</v>
       </c>
       <c r="B79" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C79" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D79" s="5">
-        <v>4027.65</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D79" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>4329</v>
+        <v>4537</v>
       </c>
       <c r="B80" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C80" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D80" s="5">
-        <v>4293</v>
+        <v>0.66003000000000001</v>
+      </c>
+      <c r="D80" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>4330</v>
+        <v>4432</v>
       </c>
       <c r="B81" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C81" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D81" s="5">
-        <v>3888.15</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D81" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>4331</v>
+        <v>4433</v>
       </c>
       <c r="B82" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C82" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D82" s="5">
-        <v>4062.75</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D82" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>4332</v>
+        <v>4434</v>
       </c>
       <c r="B83" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C83" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D83" s="5">
-        <v>3979.95</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D83" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4333</v>
+        <v>4452</v>
       </c>
       <c r="B84" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C84" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D84" s="5">
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D84" s="4">
         <v>3801.6</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4334</v>
+        <v>4453</v>
       </c>
       <c r="B85" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C85" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D85" s="5">
-        <v>3801.9</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D85" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>4336</v>
+        <v>4468</v>
       </c>
       <c r="B86" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C86" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D86" s="5">
-        <v>3888.15</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D86" s="4">
+        <v>1350</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>4368</v>
+        <v>4469</v>
       </c>
       <c r="B87" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C87" s="2">
-        <v>0.64204000000000006</v>
-      </c>
-      <c r="D87" s="5">
-        <v>3801.6</v>
+        <v>0.66220000000000001</v>
+      </c>
+      <c r="D87" s="4">
+        <v>1800.9</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>4345</v>
+        <v>4335</v>
       </c>
       <c r="B88" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C88" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D88" s="5">
-        <v>3885.22</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D88" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>4350</v>
+        <v>4359</v>
       </c>
       <c r="B89" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C89" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D89" s="5">
-        <v>3888.15</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D89" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>4353</v>
+        <v>4391</v>
       </c>
       <c r="B90" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C90" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D90" s="5">
-        <v>3801.9</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D90" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>4358</v>
+        <v>4422</v>
       </c>
       <c r="B91" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C91" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D91" s="5">
-        <v>3801.6</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D91" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>4360</v>
+        <v>4423</v>
       </c>
       <c r="B92" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C92" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D92" s="5">
-        <v>3801.6</v>
+        <v>0.66144000000000003</v>
+      </c>
+      <c r="D92" s="4">
+        <v>3801.9</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>4361</v>
+        <v>4424</v>
       </c>
       <c r="B93" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C93" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D93" s="5">
-        <v>3801.6</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D93" s="4">
+        <v>4187.7</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>4388</v>
+        <v>4425</v>
       </c>
       <c r="B94" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C94" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D94" s="5">
-        <v>4101.45</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D94" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>4392</v>
+        <v>4426</v>
       </c>
       <c r="B95" s="3">
-        <v>45890</v>
+        <v>45911</v>
       </c>
       <c r="C95" s="2">
-        <v>0.6573</v>
-      </c>
-      <c r="D95" s="5">
-        <v>3884.7</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D95" s="4">
+        <v>4114.95</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>4412</v>
+        <v>4427</v>
       </c>
       <c r="B96" s="3">
-        <v>45897</v>
+        <v>45911</v>
       </c>
       <c r="C96" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D96" s="5">
-        <v>7603.2</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D96" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>4413</v>
+        <v>4483</v>
       </c>
       <c r="B97" s="3">
-        <v>45897</v>
+        <v>45911</v>
       </c>
       <c r="C97" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D97" s="5">
-        <v>7603.2</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D97" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>4414</v>
+        <v>4484</v>
       </c>
       <c r="B98" s="3">
-        <v>45897</v>
+        <v>45911</v>
       </c>
       <c r="C98" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D98" s="5">
-        <v>7603.2</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D98" s="4">
+        <v>3801.9</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>4415</v>
+        <v>4485</v>
       </c>
       <c r="B99" s="3">
-        <v>45897</v>
+        <v>45911</v>
       </c>
       <c r="C99" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D99" s="5">
-        <v>3801.6</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D99" s="4">
+        <v>4158</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>4435</v>
+        <v>4486</v>
       </c>
       <c r="B100" s="3">
-        <v>45897</v>
+        <v>45911</v>
       </c>
       <c r="C100" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D100" s="5">
-        <v>3801.6</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D100" s="4">
+        <v>4279.5</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>4429</v>
+        <v>4487</v>
       </c>
       <c r="B101" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C101" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D101" s="5">
-        <v>7350</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D101" s="4">
+        <v>3884.7</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>4430</v>
+        <v>4488</v>
       </c>
       <c r="B102" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C102" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D102" s="5">
-        <v>7127.9</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D102" s="4">
+        <v>3979.95</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>4431</v>
+        <v>4489</v>
       </c>
       <c r="B103" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C103" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D103" s="5">
-        <v>7127.9</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D103" s="4">
+        <v>3979.95</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>4448</v>
+        <v>4490</v>
       </c>
       <c r="B104" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C104" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D104" s="5">
-        <v>7350</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D104" s="4">
+        <v>4158</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>4449</v>
+        <v>4491</v>
       </c>
       <c r="B105" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C105" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D105" s="5">
-        <v>7350</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D105" s="4">
+        <v>3979.95</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>4450</v>
+        <v>4492</v>
       </c>
       <c r="B106" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C106" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D106" s="5">
-        <v>7350</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D106" s="4">
+        <v>4066.2</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>4451</v>
+        <v>4493</v>
       </c>
       <c r="B107" s="3">
-        <v>45898</v>
+        <v>45911</v>
       </c>
       <c r="C107" s="2">
-        <v>0.62894000000000005</v>
-      </c>
-      <c r="D107" s="5">
-        <v>7350</v>
+        <v>0.66139000000000003</v>
+      </c>
+      <c r="D107" s="4">
+        <v>4158</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>4292</v>
+        <v>4527</v>
       </c>
       <c r="B108" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C108" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D108" s="5">
-        <v>3801.6</v>
+        <v>0.66390000000000005</v>
+      </c>
+      <c r="D108" s="4">
+        <v>7080</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>4352</v>
+        <v>4538</v>
       </c>
       <c r="B109" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C109" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D109" s="5">
-        <v>4293</v>
+        <v>0.66393999999999997</v>
+      </c>
+      <c r="D109" s="4">
+        <v>7350</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>4354</v>
+        <v>4470</v>
       </c>
       <c r="B110" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C110" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D110" s="5">
-        <v>4374</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D110" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>4355</v>
+        <v>4471</v>
       </c>
       <c r="B111" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C111" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D111" s="5">
-        <v>3801.6</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D111" s="4">
+        <v>7603.2</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>4356</v>
+        <v>4472</v>
       </c>
       <c r="B112" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C112" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D112" s="5">
-        <v>3979.95</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D112" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>4357</v>
+        <v>4478</v>
       </c>
       <c r="B113" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C113" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D113" s="5">
-        <v>3979.95</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D113" s="4">
+        <v>2700</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>4389</v>
+        <v>4539</v>
       </c>
       <c r="B114" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C114" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D114" s="5">
-        <v>4066.2</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D114" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>4390</v>
+        <v>4540</v>
       </c>
       <c r="B115" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C115" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D115" s="5">
-        <v>3801.9</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D115" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>4209</v>
+        <v>4541</v>
       </c>
       <c r="B116" s="3">
-        <v>45848</v>
+        <v>45918</v>
       </c>
       <c r="C116" s="2">
-        <v>0.62860000000000005</v>
-      </c>
-      <c r="D116" s="5">
-        <v>4184.25</v>
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D116" s="4">
+        <v>3801.6</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>4231</v>
+        <v>4542</v>
       </c>
       <c r="B117" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C117" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D117" s="5">
+        <v>0.66325999999999996</v>
+      </c>
+      <c r="D117" s="4">
         <v>3801.6</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>4232</v>
+        <v>4543</v>
       </c>
       <c r="B118" s="3">
-        <v>45898</v>
+        <v>45918</v>
       </c>
       <c r="C118" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D118" s="5">
+        <v>0.66457999999999995</v>
+      </c>
+      <c r="D118" s="4">
         <v>3801.6</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>4209</v>
+        <v>4441</v>
       </c>
       <c r="B119" s="3">
-        <v>45848</v>
+        <v>45918</v>
       </c>
       <c r="C119" s="2">
-        <v>0.65766999999999998</v>
-      </c>
-      <c r="D119" s="5">
-        <v>9763.25</v>
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D119" s="4">
+        <v>4293</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A120" s="2"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="4"/>
+      <c r="A120" s="2">
+        <v>4442</v>
+      </c>
+      <c r="B120" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C120" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D120" s="4">
+        <v>3888.15</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="2"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="4"/>
+      <c r="A121" s="2">
+        <v>4443</v>
+      </c>
+      <c r="B121" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C121" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D121" s="4">
+        <v>3979.95</v>
+      </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A122" s="2"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="4"/>
+      <c r="A122" s="2">
+        <v>4444</v>
+      </c>
+      <c r="B122" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C122" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D122" s="4">
+        <v>3979.95</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A123" s="2"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="4"/>
+      <c r="A123" s="2">
+        <v>4445</v>
+      </c>
+      <c r="B123" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C123" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D123" s="4">
+        <v>3979.95</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A124" s="2"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="4"/>
+      <c r="A124" s="2">
+        <v>4446</v>
+      </c>
+      <c r="B124" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C124" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D124" s="4">
+        <v>4066.2</v>
+      </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A125" s="2"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="4"/>
+      <c r="A125" s="2">
+        <v>4447</v>
+      </c>
+      <c r="B125" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C125" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D125" s="4">
+        <v>3801.6</v>
+      </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A126" s="2"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="4"/>
+      <c r="A126" s="2">
+        <v>4460</v>
+      </c>
+      <c r="B126" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C126" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D126" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A127" s="2"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="4"/>
+      <c r="A127" s="2">
+        <v>4464</v>
+      </c>
+      <c r="B127" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C127" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D127" s="4">
+        <v>3888.15</v>
+      </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A128" s="2"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="4"/>
+      <c r="A128" s="2">
+        <v>4465</v>
+      </c>
+      <c r="B128" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C128" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D128" s="4">
+        <v>3801.6</v>
+      </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A129" s="2"/>
-      <c r="B129" s="3"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="4"/>
+      <c r="A129" s="2">
+        <v>4467</v>
+      </c>
+      <c r="B129" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C129" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D129" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" s="2"/>
-      <c r="B130" s="3"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="4"/>
+      <c r="A130" s="2">
+        <v>4495</v>
+      </c>
+      <c r="B130" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C130" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D130" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A131" s="2"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="4"/>
+      <c r="A131" s="2">
+        <v>4496</v>
+      </c>
+      <c r="B131" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C131" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D131" s="4">
+        <v>4293</v>
+      </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A132" s="2"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="4"/>
+      <c r="A132" s="2">
+        <v>4498</v>
+      </c>
+      <c r="B132" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C132" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D132" s="4">
+        <v>4252.5</v>
+      </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A133" s="2"/>
-      <c r="B133" s="3"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="4"/>
+      <c r="A133" s="2">
+        <v>4499</v>
+      </c>
+      <c r="B133" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C133" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D133" s="4">
+        <v>3979.95</v>
+      </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A134" s="2"/>
-      <c r="B134" s="3"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="4"/>
+      <c r="A134" s="2">
+        <v>4505</v>
+      </c>
+      <c r="B134" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C134" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D134" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A135" s="2"/>
-      <c r="B135" s="3"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="4"/>
+      <c r="A135" s="2">
+        <v>4506</v>
+      </c>
+      <c r="B135" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C135" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D135" s="4">
+        <v>4114.95</v>
+      </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A136" s="2"/>
-      <c r="B136" s="3"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="4"/>
+      <c r="A136" s="2">
+        <v>4520</v>
+      </c>
+      <c r="B136" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C136" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D136" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="2"/>
-      <c r="B137" s="3"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="4"/>
+      <c r="A137" s="2">
+        <v>4521</v>
+      </c>
+      <c r="B137" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C137" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D137" s="4">
+        <v>4158</v>
+      </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="2"/>
-      <c r="B138" s="3"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="4"/>
+      <c r="A138" s="2">
+        <v>4522</v>
+      </c>
+      <c r="B138" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C138" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D138" s="4">
+        <v>4137.34</v>
+      </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" s="2"/>
-      <c r="B139" s="3"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="4"/>
+      <c r="A139" s="2">
+        <v>4530</v>
+      </c>
+      <c r="B139" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C139" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D139" s="4">
+        <v>3801.6</v>
+      </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" s="2"/>
-      <c r="B140" s="3"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="4"/>
+      <c r="A140" s="2">
+        <v>4531</v>
+      </c>
+      <c r="B140" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C140" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D140" s="4">
+        <v>3844.92</v>
+      </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" s="2"/>
-      <c r="B141" s="3"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="4"/>
+      <c r="A141" s="2">
+        <v>4532</v>
+      </c>
+      <c r="B141" s="3">
+        <v>45918</v>
+      </c>
+      <c r="C141" s="2">
+        <v>0.66420000000000001</v>
+      </c>
+      <c r="D141" s="4">
+        <v>4114.95</v>
+      </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A142" s="2"/>
-      <c r="B142" s="3"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="4"/>
+      <c r="A142" s="2">
+        <v>3</v>
+      </c>
+      <c r="B142" s="3">
+        <v>45923</v>
+      </c>
+      <c r="C142" s="2">
+        <v>0.66078999999999999</v>
+      </c>
+      <c r="D142" s="4">
+        <v>10350</v>
+      </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" s="2"/>
-      <c r="B143" s="3"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="4"/>
+      <c r="A143" s="2">
+        <v>4</v>
+      </c>
+      <c r="B143" s="3">
+        <v>45923</v>
+      </c>
+      <c r="C143" s="2">
+        <v>0.66080000000000005</v>
+      </c>
+      <c r="D143" s="4">
+        <v>1040</v>
+      </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" s="2"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="4"/>
+      <c r="A144" s="2">
+        <v>5</v>
+      </c>
+      <c r="B144" s="3">
+        <v>45923</v>
+      </c>
+      <c r="C144" s="2">
+        <v>0.66078999999999999</v>
+      </c>
+      <c r="D144" s="4">
+        <v>10350</v>
+      </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
       <c r="J144" s="2"/>
     </row>
-    <row r="145" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C145" s="2"/>
-    </row>
-    <row r="146" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C146" s="2"/>
-    </row>
-    <row r="147" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C147" s="2"/>
-    </row>
-    <row r="148" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C148" s="2"/>
-    </row>
-    <row r="149" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C149" s="2"/>
-    </row>
-    <row r="150" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C150" s="2"/>
-    </row>
-    <row r="151" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C151" s="2"/>
-    </row>
-    <row r="152" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C152" s="2"/>
-    </row>
-    <row r="153" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C153" s="2"/>
-    </row>
-    <row r="154" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C154" s="2"/>
-    </row>
-    <row r="155" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145" s="2">
+        <v>6</v>
+      </c>
+      <c r="B145" s="3">
+        <v>45923</v>
+      </c>
+      <c r="C145" s="2">
+        <v>0.66080000000000005</v>
+      </c>
+      <c r="D145" s="4">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146" s="2">
+        <v>4428</v>
+      </c>
+      <c r="B146" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C146" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D146" s="4">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147" s="2">
+        <v>4494</v>
+      </c>
+      <c r="B147" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C147" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D147" s="4">
+        <v>3979.95</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148" s="2">
+        <v>4500</v>
+      </c>
+      <c r="B148" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C148" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D148" s="4">
+        <v>4066.2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149" s="2">
+        <v>4501</v>
+      </c>
+      <c r="B149" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C149" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D149" s="4">
+        <v>4252.5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150" s="2">
+        <v>4518</v>
+      </c>
+      <c r="B150" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C150" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D150" s="4">
+        <v>3675.82</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151" s="2">
+        <v>4519</v>
+      </c>
+      <c r="B151" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C151" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D151" s="4">
+        <v>3972.73</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152" s="2">
+        <v>4535</v>
+      </c>
+      <c r="B152" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C152" s="2">
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D152" s="4">
+        <v>2241.14</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153" s="2">
+        <v>7</v>
+      </c>
+      <c r="B153" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C153" s="2">
+        <v>0.65937000000000001</v>
+      </c>
+      <c r="D153" s="4">
+        <v>14204.8</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154" s="2">
+        <v>4299</v>
+      </c>
+      <c r="B154" s="3">
+        <v>45925</v>
+      </c>
+      <c r="C154" s="2">
+        <v>0.62849999999999995</v>
+      </c>
+      <c r="D154" s="4">
+        <v>14586</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C155" s="2"/>
     </row>
-    <row r="156" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C156" s="2"/>
     </row>
-    <row r="157" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C157" s="2"/>
     </row>
-    <row r="158" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C158" s="2"/>
     </row>
-    <row r="159" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C159" s="2"/>
     </row>
-    <row r="160" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C160" s="2"/>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
latest trade finance & monthly DP information for supplier info
</commit_message>
<xml_diff>
--- a/H2coco/PO.xlsx
+++ b/H2coco/PO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/Github/XeroAPI/H2coco/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A21942A-2333-D54C-8CF0-5EBB68EB9217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B386559C-50B8-A140-827D-9013196FD217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="34200" windowHeight="21360" xr2:uid="{4B9AE9D0-272D-6147-B144-109295B6F9E3}"/>
   </bookViews>
@@ -444,8 +444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB96091-FFF7-FA49-AAE0-56AC976AE7FD}">
   <dimension ref="A1:J996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScale="114" workbookViewId="0">
-      <selection activeCell="H125" sqref="H125"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="114" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -469,163 +469,163 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>4169</v>
+        <v>4228</v>
       </c>
       <c r="B2" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C2" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D2" s="5">
-        <v>7935</v>
+        <v>7603.2</v>
       </c>
       <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>4173</v>
+        <v>4230</v>
       </c>
       <c r="B3" s="3">
-        <v>45834</v>
+        <v>45848</v>
       </c>
       <c r="C3" s="2">
-        <v>0.65142</v>
+        <v>0.62860000000000005</v>
       </c>
       <c r="D3" s="5">
-        <v>7935</v>
+        <v>7603.2</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>4227</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
-        <v>45848</v>
+        <v>45854</v>
       </c>
       <c r="C4" s="2">
-        <v>0.62860000000000005</v>
+        <v>0.65175000000000005</v>
       </c>
       <c r="D4" s="5">
-        <v>7603.2</v>
+        <v>11025</v>
       </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4228</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3">
-        <v>45848</v>
+        <v>45854</v>
       </c>
       <c r="C5" s="2">
-        <v>0.62860000000000005</v>
+        <v>0.65176000000000001</v>
       </c>
       <c r="D5" s="5">
-        <v>7603.2</v>
+        <v>1040</v>
       </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>4229</v>
+        <v>4178</v>
       </c>
       <c r="B6" s="3">
-        <v>45848</v>
+        <v>45869</v>
       </c>
       <c r="C6" s="2">
-        <v>0.62860000000000005</v>
+        <v>0.62870000000000004</v>
       </c>
       <c r="D6" s="5">
-        <v>7603.2</v>
+        <v>3967.5</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>4230</v>
+        <v>4349</v>
       </c>
       <c r="B7" s="3">
-        <v>45848</v>
+        <v>45883</v>
       </c>
       <c r="C7" s="2">
-        <v>0.62860000000000005</v>
+        <v>0.65759000000000001</v>
       </c>
       <c r="D7" s="5">
-        <v>7603.2</v>
+        <v>4062.75</v>
       </c>
       <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>4234</v>
       </c>
       <c r="B8" s="3">
-        <v>45854</v>
+        <v>45890</v>
       </c>
       <c r="C8" s="2">
-        <v>0.65175000000000005</v>
+        <v>0.6573</v>
       </c>
       <c r="D8" s="5">
-        <v>11025</v>
+        <v>3801.6</v>
       </c>
       <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>2</v>
+        <v>4333</v>
       </c>
       <c r="B9" s="3">
-        <v>45854</v>
+        <v>45890</v>
       </c>
       <c r="C9" s="2">
-        <v>0.65176000000000001</v>
+        <v>0.6573</v>
       </c>
       <c r="D9" s="5">
-        <v>1040</v>
+        <v>3801.6</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>4215</v>
+        <v>4358</v>
       </c>
       <c r="B10" s="3">
-        <v>45855</v>
+        <v>45890</v>
       </c>
       <c r="C10" s="2">
-        <v>0.65678000000000003</v>
+        <v>0.6573</v>
       </c>
       <c r="D10" s="5">
-        <v>4293</v>
+        <v>3801.6</v>
       </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>4213</v>
+        <v>4392</v>
       </c>
       <c r="B11" s="3">
-        <v>45862</v>
+        <v>45890</v>
       </c>
       <c r="C11" s="2">
-        <v>0.65963000000000005</v>
+        <v>0.6573</v>
       </c>
       <c r="D11" s="5">
-        <v>3967.5</v>
+        <v>3884.7</v>
       </c>
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>4296</v>
+        <v>4292</v>
       </c>
       <c r="B12" s="3">
-        <v>45869</v>
+        <v>45898</v>
       </c>
       <c r="C12" s="2">
-        <v>0.65669999999999995</v>
+        <v>0.65766999999999998</v>
       </c>
       <c r="D12" s="5">
         <v>3801.6</v>
@@ -634,73 +634,73 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>4178</v>
+        <v>4354</v>
       </c>
       <c r="B13" s="3">
-        <v>45869</v>
+        <v>45898</v>
       </c>
       <c r="C13" s="2">
-        <v>0.62870000000000004</v>
+        <v>0.65766999999999998</v>
       </c>
       <c r="D13" s="5">
-        <v>3967.5</v>
+        <v>4374</v>
       </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>4251</v>
+        <v>4394</v>
       </c>
       <c r="B14" s="3">
-        <v>45869</v>
+        <v>45904</v>
       </c>
       <c r="C14" s="2">
-        <v>0.62870000000000004</v>
+        <v>0.65197000000000005</v>
       </c>
       <c r="D14" s="5">
-        <v>4238.25</v>
+        <v>3801.6</v>
       </c>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>4270</v>
+        <v>4526</v>
       </c>
       <c r="B15" s="3">
-        <v>45869</v>
+        <v>45911</v>
       </c>
       <c r="C15" s="2">
-        <v>0.62870000000000004</v>
+        <v>0.66003000000000001</v>
       </c>
       <c r="D15" s="5">
-        <v>4293</v>
+        <v>7146.5</v>
       </c>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>4273</v>
+        <v>4452</v>
       </c>
       <c r="B16" s="3">
-        <v>45869</v>
+        <v>45911</v>
       </c>
       <c r="C16" s="2">
-        <v>0.62870000000000004</v>
+        <v>0.66220000000000001</v>
       </c>
       <c r="D16" s="5">
-        <v>3967.5</v>
+        <v>3801.6</v>
       </c>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>4310</v>
+        <v>4335</v>
       </c>
       <c r="B17" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C17" s="2">
-        <v>0.62877000000000005</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D17" s="5">
         <v>3801.6</v>
@@ -709,13 +709,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>4312</v>
+        <v>4359</v>
       </c>
       <c r="B18" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C18" s="2">
-        <v>0.65251000000000003</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D18" s="5">
         <v>3801.6</v>
@@ -723,55 +723,55 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>4313</v>
+        <v>4424</v>
       </c>
       <c r="B19" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C19" s="2">
-        <v>0.65251000000000003</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D19" s="5">
-        <v>3801.6</v>
+        <v>4187.7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>4290</v>
+        <v>4425</v>
       </c>
       <c r="B20" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C20" s="2">
-        <v>0.65739999999999998</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D20" s="5">
-        <v>2254.5</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>4291</v>
+        <v>4487</v>
       </c>
       <c r="B21" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C21" s="2">
-        <v>0.65739999999999998</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D21" s="5">
-        <v>3979.95</v>
+        <v>3884.7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>4301</v>
+        <v>4489</v>
       </c>
       <c r="B22" s="3">
-        <v>45876</v>
+        <v>45911</v>
       </c>
       <c r="C22" s="2">
-        <v>0.65739999999999998</v>
+        <v>0.66139000000000003</v>
       </c>
       <c r="D22" s="5">
         <v>3979.95</v>
@@ -779,419 +779,419 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>4326</v>
+        <v>4527</v>
       </c>
       <c r="B23" s="3">
-        <v>45876</v>
+        <v>45918</v>
       </c>
       <c r="C23" s="2">
-        <v>0.65739999999999998</v>
+        <v>0.66390000000000005</v>
       </c>
       <c r="D23" s="5">
-        <v>4157.25</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>4362</v>
+        <v>4470</v>
       </c>
       <c r="B24" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C24" s="2">
-        <v>0.629</v>
+        <v>0.66325999999999996</v>
       </c>
       <c r="D24" s="5">
-        <v>7603.2</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>4363</v>
+        <v>4540</v>
       </c>
       <c r="B25" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C25" s="2">
-        <v>0.629</v>
+        <v>0.66325999999999996</v>
       </c>
       <c r="D25" s="5">
-        <v>7603.2</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>4364</v>
+        <v>4441</v>
       </c>
       <c r="B26" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C26" s="2">
-        <v>0.629</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D26" s="5">
-        <v>7603.2</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>4365</v>
+        <v>4442</v>
       </c>
       <c r="B27" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C27" s="2">
-        <v>0.629</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D27" s="5">
-        <v>7603.2</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>4366</v>
+        <v>4443</v>
       </c>
       <c r="B28" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C28" s="2">
-        <v>0.629</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D28" s="5">
-        <v>7603.2</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>4306</v>
+        <v>4444</v>
       </c>
       <c r="B29" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C29" s="2">
-        <v>0.65759000000000001</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D29" s="5">
-        <v>3884.7</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>4349</v>
+        <v>4446</v>
       </c>
       <c r="B30" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C30" s="2">
-        <v>0.65759000000000001</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D30" s="5">
-        <v>4062.75</v>
+        <v>4066.2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>4409</v>
+        <v>4447</v>
       </c>
       <c r="B31" s="3">
-        <v>45883</v>
+        <v>45918</v>
       </c>
       <c r="C31" s="2">
-        <v>0.65764999999999996</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D31" s="5">
-        <v>7127.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>4234</v>
+        <v>4464</v>
       </c>
       <c r="B32" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C32" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D32" s="5">
-        <v>3801.6</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>4329</v>
+        <v>4465</v>
       </c>
       <c r="B33" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C33" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D33" s="5">
-        <v>4293</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>4330</v>
+        <v>4495</v>
       </c>
       <c r="B34" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C34" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D34" s="5">
-        <v>3888.15</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>4331</v>
+        <v>4496</v>
       </c>
       <c r="B35" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C35" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D35" s="5">
-        <v>4062.75</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>4332</v>
+        <v>4498</v>
       </c>
       <c r="B36" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C36" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D36" s="5">
-        <v>3979.95</v>
+        <v>4252.5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>4333</v>
+        <v>4499</v>
       </c>
       <c r="B37" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C37" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D37" s="5">
-        <v>3801.6</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>4334</v>
+        <v>4505</v>
       </c>
       <c r="B38" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C38" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D38" s="5">
-        <v>3801.9</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>4336</v>
+        <v>4506</v>
       </c>
       <c r="B39" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C39" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D39" s="5">
-        <v>3888.15</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>4345</v>
+        <v>4530</v>
       </c>
       <c r="B40" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C40" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D40" s="5">
-        <v>3885.22</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>4350</v>
+        <v>4532</v>
       </c>
       <c r="B41" s="3">
-        <v>45890</v>
+        <v>45918</v>
       </c>
       <c r="C41" s="2">
-        <v>0.6573</v>
+        <v>0.66420000000000001</v>
       </c>
       <c r="D41" s="5">
-        <v>3888.15</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>4353</v>
+        <v>3</v>
       </c>
       <c r="B42" s="3">
-        <v>45890</v>
+        <v>45923</v>
       </c>
       <c r="C42" s="2">
-        <v>0.6573</v>
+        <v>0.66078999999999999</v>
       </c>
       <c r="D42" s="5">
-        <v>3801.9</v>
+        <v>10350</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>4358</v>
+        <v>4</v>
       </c>
       <c r="B43" s="3">
-        <v>45890</v>
+        <v>45923</v>
       </c>
       <c r="C43" s="2">
-        <v>0.6573</v>
+        <v>0.66080000000000005</v>
       </c>
       <c r="D43" s="5">
-        <v>3801.6</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>4361</v>
+        <v>5</v>
       </c>
       <c r="B44" s="3">
-        <v>45890</v>
+        <v>45923</v>
       </c>
       <c r="C44" s="2">
-        <v>0.6573</v>
+        <v>0.66078999999999999</v>
       </c>
       <c r="D44" s="5">
-        <v>3801.6</v>
+        <v>10350</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>4388</v>
+        <v>6</v>
       </c>
       <c r="B45" s="3">
-        <v>45890</v>
+        <v>45923</v>
       </c>
       <c r="C45" s="2">
-        <v>0.6573</v>
+        <v>0.66080000000000005</v>
       </c>
       <c r="D45" s="5">
-        <v>4101.45</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>4392</v>
+        <v>4501</v>
       </c>
       <c r="B46" s="3">
-        <v>45890</v>
+        <v>45925</v>
       </c>
       <c r="C46" s="2">
-        <v>0.6573</v>
+        <v>0.65869999999999995</v>
       </c>
       <c r="D46" s="5">
-        <v>3884.7</v>
+        <v>4252.5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>4412</v>
+        <v>4518</v>
       </c>
       <c r="B47" s="3">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="C47" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.65869999999999995</v>
       </c>
       <c r="D47" s="5">
-        <v>7603.2</v>
+        <v>3675.82</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>4413</v>
+        <v>4519</v>
       </c>
       <c r="B48" s="3">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="C48" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.65869999999999995</v>
       </c>
       <c r="D48" s="5">
-        <v>7603.2</v>
+        <v>3972.73</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>4414</v>
+        <v>4535</v>
       </c>
       <c r="B49" s="3">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="C49" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.65869999999999995</v>
       </c>
       <c r="D49" s="5">
-        <v>7603.2</v>
+        <v>2241.14</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>4415</v>
+        <v>7</v>
       </c>
       <c r="B50" s="3">
-        <v>45897</v>
+        <v>45925</v>
       </c>
       <c r="C50" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.65937000000000001</v>
       </c>
       <c r="D50" s="5">
-        <v>3801.6</v>
+        <v>14204.8</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>4435</v>
+        <v>4502</v>
       </c>
       <c r="B51" s="3">
-        <v>45897</v>
+        <v>45932</v>
       </c>
       <c r="C51" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D51" s="5">
-        <v>3801.6</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>4231</v>
+        <v>4504</v>
       </c>
       <c r="B52" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C52" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D52" s="5">
         <v>3801.6</v>
@@ -1199,97 +1199,97 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>4429</v>
+        <v>4507</v>
       </c>
       <c r="B53" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C53" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D53" s="5">
-        <v>7350</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>4430</v>
+        <v>4508</v>
       </c>
       <c r="B54" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C54" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D54" s="5">
-        <v>7127.9</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>4431</v>
+        <v>4509</v>
       </c>
       <c r="B55" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C55" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D55" s="4">
-        <v>7127.9</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>4448</v>
+        <v>4510</v>
       </c>
       <c r="B56" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C56" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66049999999999998</v>
       </c>
       <c r="D56" s="4">
-        <v>7350</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>4449</v>
+        <v>4572</v>
       </c>
       <c r="B57" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C57" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66024000000000005</v>
       </c>
       <c r="D57" s="4">
-        <v>7350</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>4450</v>
+        <v>4574</v>
       </c>
       <c r="B58" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C58" s="2">
-        <v>0.62894000000000005</v>
+        <v>0.66024000000000005</v>
       </c>
       <c r="D58" s="4">
-        <v>7350</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>4292</v>
+        <v>4576</v>
       </c>
       <c r="B59" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C59" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.66024000000000005</v>
       </c>
       <c r="D59" s="4">
         <v>3801.6</v>
@@ -1297,125 +1297,125 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>4352</v>
+        <v>4577</v>
       </c>
       <c r="B60" s="3">
-        <v>45898</v>
+        <v>45932</v>
       </c>
       <c r="C60" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.66024000000000005</v>
       </c>
       <c r="D60" s="4">
-        <v>4293</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>4354</v>
+        <v>4462</v>
       </c>
       <c r="B61" s="3">
-        <v>45898</v>
+        <v>45939</v>
       </c>
       <c r="C61" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D61" s="4">
-        <v>4374</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>4355</v>
+        <v>4463</v>
       </c>
       <c r="B62" s="3">
-        <v>45898</v>
+        <v>45939</v>
       </c>
       <c r="C62" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D62" s="4">
-        <v>3801.6</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>4356</v>
+        <v>4553</v>
       </c>
       <c r="B63" s="3">
-        <v>45898</v>
+        <v>45939</v>
       </c>
       <c r="C63" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D63" s="4">
-        <v>3979.95</v>
+        <v>4066.2</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>4389</v>
+        <v>4554</v>
       </c>
       <c r="B64" s="3">
-        <v>45898</v>
+        <v>45939</v>
       </c>
       <c r="C64" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D64" s="4">
-        <v>4066.2</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>4390</v>
+        <v>4555</v>
       </c>
       <c r="B65" s="3">
-        <v>45898</v>
+        <v>45939</v>
       </c>
       <c r="C65" s="2">
-        <v>0.65766999999999998</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D65" s="4">
-        <v>3801.9</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>4351</v>
+        <v>4556</v>
       </c>
       <c r="B66" s="3">
-        <v>45904</v>
+        <v>45939</v>
       </c>
       <c r="C66" s="2">
-        <v>0.65197000000000005</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D66" s="4">
-        <v>4293</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>4393</v>
+        <v>4623</v>
       </c>
       <c r="B67" s="3">
-        <v>45904</v>
+        <v>45939</v>
       </c>
       <c r="C67" s="2">
-        <v>0.65197000000000005</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D67" s="4">
-        <v>3888.15</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>4394</v>
+        <v>4625</v>
       </c>
       <c r="B68" s="3">
-        <v>45904</v>
+        <v>45939</v>
       </c>
       <c r="C68" s="2">
-        <v>0.65197000000000005</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D68" s="4">
         <v>3801.6</v>
@@ -1423,139 +1423,139 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>4395</v>
+        <v>4626</v>
       </c>
       <c r="B69" s="3">
-        <v>45904</v>
+        <v>45939</v>
       </c>
       <c r="C69" s="2">
-        <v>0.65197000000000005</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D69" s="4">
-        <v>3801.6</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>4479</v>
+        <v>4628</v>
       </c>
       <c r="B70" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C70" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D70" s="4">
-        <v>7127.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>4480</v>
+        <v>4654</v>
       </c>
       <c r="B71" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C71" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D71" s="4">
-        <v>7127.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>4481</v>
+        <v>4657</v>
       </c>
       <c r="B72" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C72" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65978000000000003</v>
       </c>
       <c r="D72" s="4">
-        <v>7127.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>4482</v>
+        <v>4568</v>
       </c>
       <c r="B73" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C73" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D73" s="4">
-        <v>6832.8</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>4526</v>
+        <v>4570</v>
       </c>
       <c r="B74" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C74" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D74" s="4">
-        <v>7146.5</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>4528</v>
+        <v>4617</v>
       </c>
       <c r="B75" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C75" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D75" s="4">
-        <v>7222.5</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
-        <v>4529</v>
+        <v>4618</v>
       </c>
       <c r="B76" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C76" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D76" s="4">
-        <v>7098.25</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
-        <v>4533</v>
+        <v>4619</v>
       </c>
       <c r="B77" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C77" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D77" s="4">
-        <v>7127.9</v>
+        <v>7000.4</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
-        <v>4534</v>
+        <v>4620</v>
       </c>
       <c r="B78" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C78" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D78" s="4">
         <v>7350</v>
@@ -1563,447 +1563,447 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
-        <v>4536</v>
+        <v>4621</v>
       </c>
       <c r="B79" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C79" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65890000000000004</v>
       </c>
       <c r="D79" s="4">
-        <v>7350</v>
+        <v>7127.9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
-        <v>4537</v>
+        <v>4558</v>
       </c>
       <c r="B80" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C80" s="2">
-        <v>0.66003000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D80" s="4">
-        <v>7350</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
-        <v>4432</v>
+        <v>4559</v>
       </c>
       <c r="B81" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C81" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D81" s="4">
-        <v>3801.6</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
-        <v>4433</v>
+        <v>4560</v>
       </c>
       <c r="B82" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C82" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D82" s="4">
-        <v>3801.6</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
-        <v>4434</v>
+        <v>4562</v>
       </c>
       <c r="B83" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C83" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D83" s="4">
-        <v>3801.6</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
-        <v>4452</v>
+        <v>4567</v>
       </c>
       <c r="B84" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C84" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D84" s="4">
-        <v>3801.6</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
-        <v>4453</v>
+        <v>4583</v>
       </c>
       <c r="B85" s="3">
-        <v>45911</v>
+        <v>45939</v>
       </c>
       <c r="C85" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65790000000000004</v>
       </c>
       <c r="D85" s="4">
-        <v>3801.6</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
-        <v>4468</v>
+        <v>4512</v>
       </c>
       <c r="B86" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C86" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D86" s="4">
-        <v>1350</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
-        <v>4469</v>
+        <v>4547</v>
       </c>
       <c r="B87" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C87" s="2">
-        <v>0.66220000000000001</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D87" s="4">
-        <v>1800.9</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
-        <v>4335</v>
+        <v>4548</v>
       </c>
       <c r="B88" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C88" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D88" s="4">
-        <v>3801.6</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
-        <v>4359</v>
+        <v>4549</v>
       </c>
       <c r="B89" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C89" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65493999999999997</v>
       </c>
       <c r="D89" s="4">
-        <v>3801.6</v>
+        <v>4387.5</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
-        <v>4391</v>
+        <v>4550</v>
       </c>
       <c r="B90" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C90" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D90" s="4">
-        <v>4293</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
-        <v>4422</v>
+        <v>4551</v>
       </c>
       <c r="B91" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C91" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D91" s="4">
-        <v>4293</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
-        <v>4423</v>
+        <v>4552</v>
       </c>
       <c r="B92" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C92" s="2">
-        <v>0.66144000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D92" s="4">
-        <v>3801.9</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
-        <v>4424</v>
+        <v>4557</v>
       </c>
       <c r="B93" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C93" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D93" s="4">
-        <v>4187.7</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
-        <v>4425</v>
+        <v>4565</v>
       </c>
       <c r="B94" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C94" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D94" s="4">
-        <v>3801.6</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
-        <v>4426</v>
+        <v>4579</v>
       </c>
       <c r="B95" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C95" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D95" s="4">
-        <v>4114.95</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
-        <v>4427</v>
+        <v>4580</v>
       </c>
       <c r="B96" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C96" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D96" s="4">
-        <v>4293</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
-        <v>4483</v>
+        <v>4581</v>
       </c>
       <c r="B97" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C97" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D97" s="4">
-        <v>4293</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
-        <v>4484</v>
+        <v>4584</v>
       </c>
       <c r="B98" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C98" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D98" s="4">
-        <v>3801.9</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
-        <v>4485</v>
+        <v>4585</v>
       </c>
       <c r="B99" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C99" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D99" s="4">
-        <v>4158</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
-        <v>4486</v>
+        <v>4587</v>
       </c>
       <c r="B100" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C100" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D100" s="4">
-        <v>4279.5</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
-        <v>4487</v>
+        <v>4588</v>
       </c>
       <c r="B101" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C101" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D101" s="4">
-        <v>3884.7</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
-        <v>4488</v>
+        <v>4589</v>
       </c>
       <c r="B102" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C102" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D102" s="4">
-        <v>3979.95</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
-        <v>4489</v>
+        <v>4590</v>
       </c>
       <c r="B103" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C103" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D103" s="4">
-        <v>3979.95</v>
+        <v>4158</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
-        <v>4490</v>
+        <v>4591</v>
       </c>
       <c r="B104" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C104" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D104" s="4">
-        <v>4158</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
-        <v>4491</v>
+        <v>4592</v>
       </c>
       <c r="B105" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C105" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D105" s="4">
-        <v>3979.95</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
-        <v>4492</v>
+        <v>4622</v>
       </c>
       <c r="B106" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C106" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D106" s="4">
-        <v>4066.2</v>
+        <v>4101.45</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
-        <v>4493</v>
+        <v>4624</v>
       </c>
       <c r="B107" s="3">
-        <v>45911</v>
+        <v>45946</v>
       </c>
       <c r="C107" s="2">
-        <v>0.66139000000000003</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D107" s="4">
-        <v>4158</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
-        <v>4527</v>
+        <v>4675</v>
       </c>
       <c r="B108" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C108" s="2">
-        <v>0.66390000000000005</v>
+        <v>0.65949000000000002</v>
       </c>
       <c r="D108" s="4">
-        <v>7080</v>
+        <v>4101.45</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
-        <v>4538</v>
+        <v>4655</v>
       </c>
       <c r="B109" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C109" s="2">
-        <v>0.66393999999999997</v>
+        <v>0.65869</v>
       </c>
       <c r="D109" s="4">
-        <v>7350</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
-        <v>4470</v>
+        <v>4656</v>
       </c>
       <c r="B110" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C110" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D110" s="4">
         <v>3801.6</v>
@@ -2011,27 +2011,27 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
-        <v>4471</v>
+        <v>4677</v>
       </c>
       <c r="B111" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C111" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D111" s="4">
-        <v>7603.2</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
-        <v>4472</v>
+        <v>4678</v>
       </c>
       <c r="B112" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C112" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D112" s="4">
         <v>3801.6</v>
@@ -2039,27 +2039,27 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
-        <v>4478</v>
+        <v>4679</v>
       </c>
       <c r="B113" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C113" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D113" s="4">
-        <v>2700</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
-        <v>4539</v>
+        <v>4680</v>
       </c>
       <c r="B114" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C114" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D114" s="4">
         <v>3801.6</v>
@@ -2067,55 +2067,55 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
-        <v>4540</v>
+        <v>4732</v>
       </c>
       <c r="B115" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C115" s="2">
-        <v>0.66325999999999996</v>
+        <v>0.65869</v>
       </c>
       <c r="D115" s="4">
-        <v>3801.6</v>
+        <v>2249.1</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
-        <v>4541</v>
+        <v>4733</v>
       </c>
       <c r="B116" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C116" s="2">
-        <v>0.66325999999999996</v>
-      </c>
-      <c r="D116" s="4">
-        <v>3801.6</v>
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D116" s="2">
+        <v>180.9</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
-        <v>4542</v>
+        <v>4734</v>
       </c>
       <c r="B117" s="3">
-        <v>45918</v>
+        <v>45946</v>
       </c>
       <c r="C117" s="2">
-        <v>0.66325999999999996</v>
-      </c>
-      <c r="D117" s="4">
-        <v>3801.6</v>
+        <v>0.65869999999999995</v>
+      </c>
+      <c r="D117" s="2">
+        <v>180.9</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
-        <v>4543</v>
+        <v>4466</v>
       </c>
       <c r="B118" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C118" s="2">
-        <v>0.66457999999999995</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D118" s="4">
         <v>3801.6</v>
@@ -2123,111 +2123,111 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
-        <v>4441</v>
+        <v>4561</v>
       </c>
       <c r="B119" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C119" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D119" s="4">
-        <v>4293</v>
+        <v>3538.08</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
-        <v>4442</v>
+        <v>4566</v>
       </c>
       <c r="B120" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C120" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D120" s="4">
-        <v>3888.15</v>
+        <v>3316.95</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
-        <v>4443</v>
+        <v>4569</v>
       </c>
       <c r="B121" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C121" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D121" s="4">
-        <v>3979.95</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
-        <v>4444</v>
+        <v>4571</v>
       </c>
       <c r="B122" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C122" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D122" s="4">
-        <v>3979.95</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
-        <v>4445</v>
+        <v>4573</v>
       </c>
       <c r="B123" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C123" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D123" s="4">
-        <v>3979.95</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
-        <v>4446</v>
+        <v>4630</v>
       </c>
       <c r="B124" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C124" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D124" s="4">
-        <v>4066.2</v>
+        <v>3979.95</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
-        <v>4447</v>
+        <v>4632</v>
       </c>
       <c r="B125" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C125" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D125" s="4">
-        <v>3801.6</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
-        <v>4460</v>
+        <v>4633</v>
       </c>
       <c r="B126" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C126" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D126" s="4">
         <v>4158</v>
@@ -2235,41 +2235,41 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="2">
-        <v>4464</v>
+        <v>4634</v>
       </c>
       <c r="B127" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C127" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D127" s="4">
-        <v>3888.15</v>
+        <v>4114.95</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="2">
-        <v>4465</v>
+        <v>4635</v>
       </c>
       <c r="B128" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C128" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D128" s="4">
-        <v>3801.6</v>
+        <v>3888.15</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129" s="2">
-        <v>4467</v>
+        <v>4636</v>
       </c>
       <c r="B129" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C129" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.66034000000000004</v>
       </c>
       <c r="D129" s="4">
         <v>4158</v>
@@ -2277,212 +2277,212 @@
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" s="2">
-        <v>4495</v>
+        <v>4399</v>
       </c>
       <c r="B130" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C130" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D130" s="4">
-        <v>4158</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131" s="2">
-        <v>4496</v>
+        <v>4400</v>
       </c>
       <c r="B131" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C131" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D131" s="4">
-        <v>4293</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" s="2">
-        <v>4498</v>
+        <v>4401</v>
       </c>
       <c r="B132" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C132" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D132" s="4">
-        <v>4252.5</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133" s="2">
-        <v>4499</v>
+        <v>4402</v>
       </c>
       <c r="B133" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C133" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D133" s="4">
-        <v>3979.95</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" s="2">
-        <v>4505</v>
+        <v>4403</v>
       </c>
       <c r="B134" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C134" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D134" s="4">
-        <v>4158</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" s="2">
-        <v>4506</v>
+        <v>4404</v>
       </c>
       <c r="B135" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C135" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D135" s="4">
-        <v>4114.95</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" s="2">
-        <v>4520</v>
+        <v>4405</v>
       </c>
       <c r="B136" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C136" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D136" s="4">
-        <v>4158</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" s="2">
-        <v>4521</v>
+        <v>4406</v>
       </c>
       <c r="B137" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C137" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64810000000000001</v>
       </c>
       <c r="D137" s="4">
-        <v>4158</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" s="2">
-        <v>4522</v>
+        <v>4407</v>
       </c>
       <c r="B138" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C138" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64815</v>
       </c>
       <c r="D138" s="4">
-        <v>4137.34</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" s="2">
-        <v>4530</v>
+        <v>4408</v>
       </c>
       <c r="B139" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C139" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.64883999999999997</v>
       </c>
       <c r="D139" s="4">
-        <v>3801.6</v>
+        <v>4375.8</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" s="2">
-        <v>4531</v>
+        <v>4713</v>
       </c>
       <c r="B140" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C140" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.6482</v>
       </c>
       <c r="D140" s="4">
-        <v>3844.92</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" s="2">
-        <v>4532</v>
+        <v>4714</v>
       </c>
       <c r="B141" s="3">
-        <v>45918</v>
+        <v>45953</v>
       </c>
       <c r="C141" s="2">
-        <v>0.66420000000000001</v>
+        <v>0.6482</v>
       </c>
       <c r="D141" s="4">
-        <v>4114.95</v>
+        <v>7603.2</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" s="2">
-        <v>3</v>
+        <v>4716</v>
       </c>
       <c r="B142" s="3">
-        <v>45923</v>
+        <v>45953</v>
       </c>
       <c r="C142" s="2">
-        <v>0.66078999999999999</v>
+        <v>0.6482</v>
       </c>
       <c r="D142" s="4">
-        <v>10350</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" s="2">
-        <v>4</v>
+        <v>4717</v>
       </c>
       <c r="B143" s="3">
-        <v>45923</v>
+        <v>45953</v>
       </c>
       <c r="C143" s="2">
-        <v>0.66080000000000005</v>
+        <v>0.6482</v>
       </c>
       <c r="D143" s="4">
-        <v>1040</v>
+        <v>3801.6</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" s="2">
-        <v>5</v>
+        <v>4670</v>
       </c>
       <c r="B144" s="3">
-        <v>45923</v>
+        <v>45953</v>
       </c>
       <c r="C144" s="2">
-        <v>0.66078999999999999</v>
+        <v>0.6482</v>
       </c>
       <c r="D144" s="4">
-        <v>10350</v>
+        <v>7127.9</v>
       </c>
       <c r="E144" s="2"/>
       <c r="F144" s="2"/>
@@ -2492,143 +2492,119 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="2">
-        <v>6</v>
+        <v>4671</v>
       </c>
       <c r="B145" s="3">
-        <v>45923</v>
+        <v>45953</v>
       </c>
       <c r="C145" s="2">
-        <v>0.66080000000000005</v>
+        <v>0.6482</v>
       </c>
       <c r="D145" s="4">
-        <v>1040</v>
+        <v>7127.9</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="2">
-        <v>4428</v>
+        <v>4672</v>
       </c>
       <c r="B146" s="3">
-        <v>45925</v>
+        <v>45953</v>
       </c>
       <c r="C146" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.6482</v>
       </c>
       <c r="D146" s="4">
-        <v>3979.95</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="2">
-        <v>4494</v>
+        <v>4673</v>
       </c>
       <c r="B147" s="3">
-        <v>45925</v>
+        <v>45953</v>
       </c>
       <c r="C147" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.6482</v>
       </c>
       <c r="D147" s="4">
-        <v>3979.95</v>
+        <v>7054.9</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="2">
-        <v>4500</v>
+        <v>4674</v>
       </c>
       <c r="B148" s="3">
-        <v>45925</v>
+        <v>45953</v>
       </c>
       <c r="C148" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.6482</v>
       </c>
       <c r="D148" s="4">
-        <v>4066.2</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="2">
-        <v>4501</v>
+        <v>4710</v>
       </c>
       <c r="B149" s="3">
-        <v>45925</v>
+        <v>45953</v>
       </c>
       <c r="C149" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.6482</v>
       </c>
       <c r="D149" s="4">
-        <v>4252.5</v>
+        <v>7350</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="2">
-        <v>4518</v>
+        <v>4711</v>
       </c>
       <c r="B150" s="3">
-        <v>45925</v>
+        <v>45953</v>
       </c>
       <c r="C150" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.6482</v>
       </c>
       <c r="D150" s="4">
-        <v>3675.82</v>
+        <v>7127.9</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="2">
-        <v>4519</v>
+        <v>4299</v>
       </c>
       <c r="B151" s="3">
         <v>45925</v>
       </c>
       <c r="C151" s="2">
-        <v>0.65869999999999995</v>
+        <v>0.62849999999999995</v>
       </c>
       <c r="D151" s="4">
-        <v>3972.73</v>
+        <v>14586</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A152" s="2">
-        <v>4535</v>
-      </c>
-      <c r="B152" s="3">
-        <v>45925</v>
-      </c>
-      <c r="C152" s="2">
-        <v>0.65869999999999995</v>
-      </c>
-      <c r="D152" s="4">
-        <v>2241.14</v>
-      </c>
+      <c r="A152" s="2"/>
+      <c r="B152" s="3"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="4"/>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A153" s="2">
-        <v>7</v>
-      </c>
-      <c r="B153" s="3">
-        <v>45925</v>
-      </c>
-      <c r="C153" s="2">
-        <v>0.65937000000000001</v>
-      </c>
-      <c r="D153" s="4">
-        <v>14204.8</v>
-      </c>
+      <c r="A153" s="2"/>
+      <c r="B153" s="3"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="4"/>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A154" s="2">
-        <v>4299</v>
-      </c>
-      <c r="B154" s="3">
-        <v>45925</v>
-      </c>
-      <c r="C154" s="2">
-        <v>0.62849999999999995</v>
-      </c>
-      <c r="D154" s="4">
-        <v>14586</v>
-      </c>
+      <c r="A154" s="2"/>
+      <c r="B154" s="3"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="4"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C155" s="2"/>

</xml_diff>